<commit_message>
Wilmamsg sent. Next: Message personalization.
</commit_message>
<xml_diff>
--- a/er-plan.xlsx
+++ b/er-plan.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="24">
   <si>
     <t>PrimusAlerts</t>
   </si>
@@ -87,6 +87,15 @@
   </si>
   <si>
     <t>PrimusAlertId</t>
+  </si>
+  <si>
+    <t>AlertReceiverId</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>AlertReceivers</t>
   </si>
 </sst>
 </file>
@@ -205,6 +214,54 @@
         <a:xfrm rot="10800000" flipV="1">
           <a:off x="2905125" y="685799"/>
           <a:ext cx="2667000" cy="219075"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector3">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:headEnd type="triangle"/>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>581026</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>495301</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>133349</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="4" name="Kulmayhdysviiva 3"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="10800000" flipV="1">
+          <a:off x="3152776" y="1076325"/>
+          <a:ext cx="5819775" cy="409574"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector3">
           <a:avLst/>
@@ -497,10 +554,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:H11"/>
+  <dimension ref="B2:L11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -508,10 +565,11 @@
     <col min="3" max="3" width="20.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="36.42578125" customWidth="1"/>
     <col min="7" max="7" width="15.5703125" customWidth="1"/>
+    <col min="11" max="11" width="16.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="1"/>
       <c r="C3" s="2" t="s">
         <v>0</v>
@@ -522,8 +580,13 @@
         <v>9</v>
       </c>
       <c r="H3" s="3"/>
-    </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="J3" s="1"/>
+      <c r="K3" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="L3" s="3"/>
+    </row>
+    <row r="4" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>1</v>
       </c>
@@ -542,8 +605,17 @@
       <c r="H4" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="J4" t="s">
+        <v>1</v>
+      </c>
+      <c r="K4" t="s">
+        <v>21</v>
+      </c>
+      <c r="L4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>3</v>
       </c>
@@ -559,8 +631,14 @@
       <c r="H5" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="K5" t="s">
+        <v>22</v>
+      </c>
+      <c r="L5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="2:12" x14ac:dyDescent="0.25">
       <c r="C6" t="s">
         <v>4</v>
       </c>
@@ -573,8 +651,14 @@
       <c r="H6" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="K6" t="s">
+        <v>4</v>
+      </c>
+      <c r="L6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="2:12" x14ac:dyDescent="0.25">
       <c r="C7" t="s">
         <v>6</v>
       </c>
@@ -588,7 +672,10 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>3</v>
+      </c>
       <c r="C8" t="s">
         <v>8</v>
       </c>
@@ -602,7 +689,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:12" x14ac:dyDescent="0.25">
       <c r="G9" t="s">
         <v>15</v>
       </c>
@@ -610,7 +697,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:12" x14ac:dyDescent="0.25">
       <c r="G10" t="s">
         <v>16</v>
       </c>
@@ -618,7 +705,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:12" x14ac:dyDescent="0.25">
       <c r="G11" t="s">
         <v>17</v>
       </c>

</xml_diff>